<commit_message>
Riempimento ulteriore del primo municipio+aggiusto excel
</commit_message>
<xml_diff>
--- a/ElencoLuoghi (1).xlsx
+++ b/ElencoLuoghi (1).xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr codeName="Questa_cartella_di_lavoro" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NB-CASA\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Capobianco\Desktop\Progetto Ltw\ProgettoLTW\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF867CC4-26B2-4C15-959A-8FFF69D16E78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82183C58-8D45-4E5C-B9F7-85C5583D666D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="8" activeTab="14" xr2:uid="{0B196746-07DA-4CED-8518-28D76236140F}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{0B196746-07DA-4CED-8518-28D76236140F}"/>
   </bookViews>
   <sheets>
     <sheet name="Municipio I" sheetId="15" r:id="rId1"/>
@@ -80,7 +80,7 @@
     <definedName name="DellaVittoria">'Municipio XV'!$A:$A</definedName>
     <definedName name="Don_Bosco">'Municipio VII'!$B:$B</definedName>
     <definedName name="DonBosco">#REF!</definedName>
-    <definedName name="Eroi">'Municipio I'!$J:$J</definedName>
+    <definedName name="Eroi_DellaVittoria">'Municipio I'!$J:$J</definedName>
     <definedName name="Esquilino">'Municipio I'!$E:$E</definedName>
     <definedName name="Eur">#REF!</definedName>
     <definedName name="Europa">'Municipio IX'!$A:$A</definedName>
@@ -216,7 +216,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="72">
   <si>
     <t>Mama Shelter</t>
   </si>
@@ -802,8 +802,8 @@
   <sheetPr codeName="Foglio1"/>
   <dimension ref="A1:J40"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J14" activeCellId="1" sqref="J14 J11:J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="25.77734375" defaultRowHeight="19.95" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -895,8 +895,8 @@
       <c r="I8" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="J8" s="1" t="s">
-        <v>66</v>
+      <c r="J8" s="2" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -906,29 +906,29 @@
       <c r="I9" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="J9" s="1" t="s">
-        <v>67</v>
+      <c r="J9" s="2" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="I10" s="1" t="s">
+      <c r="I10" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="J10" s="1" t="s">
-        <v>68</v>
+      <c r="J10" s="2" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="I11" s="1" t="s">
+      <c r="I11" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="J11" s="1" t="s">
+      <c r="J11" s="2" t="s">
         <v>69</v>
       </c>
     </row>
@@ -936,19 +936,28 @@
       <c r="A12" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="I12" s="1" t="s">
+      <c r="I12" s="2" t="s">
         <v>65</v>
+      </c>
+      <c r="J12" s="2" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>20</v>
       </c>
+      <c r="J13" s="2" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="14" spans="1:10" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>21</v>
       </c>
+      <c r="J14" s="2" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="15" spans="1:10" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
@@ -1076,7 +1085,7 @@
       </c>
     </row>
     <row r="40" spans="1:1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="1" t="s">
+      <c r="A40" s="2" t="s">
         <v>62</v>
       </c>
     </row>
@@ -1166,32 +1175,31 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E6EBF7D-AA9E-4B0F-B2CF-8FAF2CB36E19}">
   <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="25.77734375" defaultRowHeight="19.95" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="25.77734375" style="1"/>
+    <col min="1" max="16384" width="25.77734375" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="2" spans="1:1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="1" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="1" t="s">
         <v>50</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="0" copies="0" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Aggiunto Quartiere Parioli,Flaminio e Salario si sulla mappa che su excel + ho preparato i prossimi quartieri del municipio II :)
</commit_message>
<xml_diff>
--- a/ElencoLuoghi (1).xlsx
+++ b/ElencoLuoghi (1).xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Capobianco\Desktop\Progetto Ltw\ProgettoLTW\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82183C58-8D45-4E5C-B9F7-85C5583D666D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B75DFD11-88A6-48BB-8045-A6FC84138D72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{0B196746-07DA-4CED-8518-28D76236140F}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{0B196746-07DA-4CED-8518-28D76236140F}"/>
   </bookViews>
   <sheets>
     <sheet name="Municipio I" sheetId="15" r:id="rId1"/>
@@ -216,7 +216,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="102">
   <si>
     <t>Mama Shelter</t>
   </si>
@@ -432,6 +432,97 @@
   </si>
   <si>
     <t>Vino e Peperoncino</t>
+  </si>
+  <si>
+    <t>Duke's</t>
+  </si>
+  <si>
+    <t>Caffè Parnaso</t>
+  </si>
+  <si>
+    <t>Ercoli 1928</t>
+  </si>
+  <si>
+    <t>Bar - Caffè delle Nazioni ai Parioli</t>
+  </si>
+  <si>
+    <t>Gotha Roma</t>
+  </si>
+  <si>
+    <t>Mostò</t>
+  </si>
+  <si>
+    <t>Mediterraneo Ristorante e Giardino</t>
+  </si>
+  <si>
+    <t>Metropolita</t>
+  </si>
+  <si>
+    <t>Etablino - Caffè Due Fontane</t>
+  </si>
+  <si>
+    <t>Frisó</t>
+  </si>
+  <si>
+    <t>Cavatappi enoteca wine bar bistrot</t>
+  </si>
+  <si>
+    <t>Enoteca Flaminio Roma</t>
+  </si>
+  <si>
+    <t>Un Caffè con Te</t>
+  </si>
+  <si>
+    <t>Ristorante "Apoteca - Provviste Alimentari" - Quartiere Flaminio, Roma</t>
+  </si>
+  <si>
+    <t>Jacobà</t>
+  </si>
+  <si>
+    <t>Enoteca Parioli</t>
+  </si>
+  <si>
+    <t>Bambu’s Parioli, Roma</t>
+  </si>
+  <si>
+    <t>Palmerie Parioli</t>
+  </si>
+  <si>
+    <t>Bar Villa Glori</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dolce caffè
+</t>
+  </si>
+  <si>
+    <t>Molinari Antonio</t>
+  </si>
+  <si>
+    <t>PAPY</t>
+  </si>
+  <si>
+    <t>KABB</t>
+  </si>
+  <si>
+    <t>Gallo Bar</t>
+  </si>
+  <si>
+    <t>Dietro Le Quinte</t>
+  </si>
+  <si>
+    <t>La vineria</t>
+  </si>
+  <si>
+    <t>Sesto</t>
+  </si>
+  <si>
+    <t>Della Manna</t>
+  </si>
+  <si>
+    <t>New Age Cafè</t>
+  </si>
+  <si>
+    <t>Lo Scoiattolo Ada</t>
   </si>
 </sst>
 </file>
@@ -481,10 +572,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -802,7 +896,7 @@
   <sheetPr codeName="Foglio1"/>
   <dimension ref="A1:J40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="J14" activeCellId="1" sqref="J14 J11:J14"/>
     </sheetView>
   </sheetViews>
@@ -1206,14 +1300,128 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F808B082-454E-4962-98AB-BE6CF8AF7856}">
   <sheetPr codeName="Foglio2"/>
-  <dimension ref="A1"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G1" sqref="G1:G1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="25.77734375" defaultRowHeight="19.95" customHeight="1" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <sheetFormatPr defaultColWidth="30.77734375" defaultRowHeight="19.95" customHeight="1" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="16384" width="30.77734375" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="0" copies="0" r:id="rId1"/>
 </worksheet>

</xml_diff>